<commit_message>
Updated system compare spreadsheet
</commit_message>
<xml_diff>
--- a/support/system-compare.xlsx
+++ b/support/system-compare.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="17235" windowHeight="11055"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="17235" windowHeight="9960"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Systems" sheetId="1" r:id="rId1"/>
+    <sheet name="Conferences" sheetId="2" r:id="rId2"/>
+    <sheet name="Caltech System" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="193">
   <si>
     <t>System</t>
   </si>
@@ -220,6 +220,382 @@
   </si>
   <si>
     <t>L3 Provision (Holographic Radar)</t>
+  </si>
+  <si>
+    <t>SET CounterBomber</t>
+  </si>
+  <si>
+    <t>Microsemi - GEN 2, MobileScan</t>
+  </si>
+  <si>
+    <t>http://www.arrowmid.com/Products/pdf/BIS-WDS_GEN2_Cut_Sheet.pdf</t>
+  </si>
+  <si>
+    <t>Brijot mm-wave tech &amp; assets acquired by Microsemi Corp, July 2011</t>
+  </si>
+  <si>
+    <t>http://globenewswire.com/news-release/2011/07/19/451549/226833/en/Microsemi-Acquires-the-Technology-and-Related-Assets-From-Brijot-Imaging-Systems-Inc.html</t>
+  </si>
+  <si>
+    <t>http://www.leidos.com/products/security/counterbomber</t>
+  </si>
+  <si>
+    <t>non-imaging, video-steered radar?, 300 K</t>
+  </si>
+  <si>
+    <t>Commercial Systems</t>
+  </si>
+  <si>
+    <t>http://thz.caltech.edu/siegelpapers/Radar-MTT08.pdf</t>
+  </si>
+  <si>
+    <t>Cooper, IEEE MTT 56 (12) 2771, 2008</t>
+  </si>
+  <si>
+    <t>Penetrating 3-D Imaging at 4- and 25-m Range Using a Submillimeter-Wave Radar</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>JPL Radar</t>
+  </si>
+  <si>
+    <t>BibLaTeX key</t>
+  </si>
+  <si>
+    <t>cooper_penetrating_2008</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=4264090&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>"first submillimeter-wave imaging system that has radar ranging capabilities"</t>
+  </si>
+  <si>
+    <t>600 GHz Imaging Radar with 2 cm Range Resolution</t>
+  </si>
+  <si>
+    <t>dengler_600_2007</t>
+  </si>
+  <si>
+    <t>Dengler, MTT-S 2007</t>
+  </si>
+  <si>
+    <t>General Background</t>
+  </si>
+  <si>
+    <t>Standoff Detection of Weapons and Contraband in the 100 GHz to 1 THz Region</t>
+  </si>
+  <si>
+    <t>Appleby &amp; Wallace, IEEE Antennas &amp; Prop</t>
+  </si>
+  <si>
+    <t>appleby_standoff_2007</t>
+  </si>
+  <si>
+    <t>everybody references this</t>
+  </si>
+  <si>
+    <t>Passive Millimeter Wave Imaging</t>
+  </si>
+  <si>
+    <t>Yujiri, IEEE MTT-S</t>
+  </si>
+  <si>
+    <t>might have references to other precursor systems</t>
+  </si>
+  <si>
+    <t>http://link.springer.com/article/10.1007%2Fs10762-009-9565-8</t>
+  </si>
+  <si>
+    <t>weg_fast_2009</t>
+  </si>
+  <si>
+    <t>Fast Active THz Cameras with Ranging Capabilities</t>
+  </si>
+  <si>
+    <t>Christian am Weg, J. Infra. Mm. THz Waves</t>
+  </si>
+  <si>
+    <t>Goethe</t>
+  </si>
+  <si>
+    <t>To-Do</t>
+  </si>
+  <si>
+    <t>find most recent pub</t>
+  </si>
+  <si>
+    <t>Terahertz imaging radar with aperture synthetic techniques for object detection</t>
+  </si>
+  <si>
+    <t>Biao Zhang</t>
+  </si>
+  <si>
+    <t>Chengdu</t>
+  </si>
+  <si>
+    <t>240 GHz, not nearly as mature as JPL</t>
+  </si>
+  <si>
+    <t>645 GHz, 300 GHz, not nearly as mature as JPL radar</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=4665482&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>Concealed object contrast enhancement using radar methods in a submillimeter-wave active imager</t>
+  </si>
+  <si>
+    <t>Comparison and design of 3-D terahertz pulsed imaging systems</t>
+  </si>
+  <si>
+    <t>Meng Zhang, ICMMT</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6230390&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>pulsed, not radar. Useful ref to earlier active systems</t>
+  </si>
+  <si>
+    <t>zhang_comparison_2012</t>
+  </si>
+  <si>
+    <t>zhang_terahertz_2013</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6005328&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>cooper_thz_2011</t>
+  </si>
+  <si>
+    <t>THz Imaging Radar for Standoff Personnel Screening</t>
+  </si>
+  <si>
+    <t>petkie_multimode_2012</t>
+  </si>
+  <si>
+    <t>Multimode illumination in the terahertz for elimination of target orientation requirements and minimization of coherent effects in active imaging systems</t>
+  </si>
+  <si>
+    <t>murrill_terahertz_2008</t>
+  </si>
+  <si>
+    <t>Terahertz imaging system performance model for concealed-weapon identification</t>
+  </si>
+  <si>
+    <t>may explain why active images don't look as good as you would think</t>
+  </si>
+  <si>
+    <t>referenced by above</t>
+  </si>
+  <si>
+    <t>d._n._bittner_passive_1987</t>
+  </si>
+  <si>
+    <t>Passive imaging with a broadband cooled detector</t>
+  </si>
+  <si>
+    <t>early (earliest?) cooled bolometer image</t>
+  </si>
+  <si>
+    <t>maybe email for more details? Can't find this online</t>
+  </si>
+  <si>
+    <t>andrews_active_2013</t>
+  </si>
+  <si>
+    <t>Active Millimeter Wave Sensor for Standoff Concealed Threat Detection</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6578195&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>A 0.32 THz SiGe 4x4 Imaging Array Using High-Efficiency On-Chip Antennas</t>
+  </si>
+  <si>
+    <t>uzunkol_0.32_2013</t>
+  </si>
+  <si>
+    <t>Uzunkol</t>
+  </si>
+  <si>
+    <t>34 pW / rt-Hz NEP, table of references to other  passive radiometric schemes</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6231669&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>garcia-pino_bifocal_2012</t>
+  </si>
+  <si>
+    <t>A Bifocal Ellipsoidal Gregorian Reflector System for THz Imaging Applications</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6146384&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>Security Pre-screening of Moving Persons Using a Rotating Multichannel W -Band Radar</t>
+  </si>
+  <si>
+    <t>hantscher_security_2012</t>
+  </si>
+  <si>
+    <t>96-99 GHz, active.</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6392315&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>72 GHz, so not standoff, but very interesting, may get to video?</t>
+  </si>
+  <si>
+    <t>Fully Electronic  E -Band Personnel Imager of 2 m^2 Aperture Based on a Multistatic Architecture</t>
+  </si>
+  <si>
+    <t>ahmed_fully_2013</t>
+  </si>
+  <si>
+    <t>another active approach, 270-330 GHz</t>
+  </si>
+  <si>
+    <t>Submillimeter-Wave Frequency Scanning System for Imaging Applications</t>
+  </si>
+  <si>
+    <t>alvarez_submillimeter-wave_2013</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6258431&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>problem at 675 GHz is apparently noise in carrier signal, not reciever</t>
+  </si>
+  <si>
+    <t>cooper_carrier_2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrier noise-limited penetration in THz radar imaging
+</t>
+  </si>
+  <si>
+    <t>read this</t>
+  </si>
+  <si>
+    <t>claim 30 FPS at 25 m standoff, neural net detection</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=5062508&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>interesting idea for increasing depth of field</t>
+  </si>
+  <si>
+    <t>mait_94-ghz_2009</t>
+  </si>
+  <si>
+    <t>94-GHz Imager With Extended Depth of Field</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpls/abs_all.jsp?arnumber=6015499</t>
+  </si>
+  <si>
+    <t>Design and Analysis of a W-Band SiGe Direct-Detection-Based Passive Imaging Receiver</t>
+  </si>
+  <si>
+    <t>gilreath_design_2011</t>
+  </si>
+  <si>
+    <t>passive, only still image of coin in envelope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference for challenges of wide field of view with steering systems? could be useful in future … </t>
+  </si>
+  <si>
+    <t>http://www.opticsinfobase.org/josab/abstract.cfm?&amp;uri=josab-25-9-1523</t>
+  </si>
+  <si>
+    <t>Active and passive imaging in the THz spectral region: phenomenology, dynamic range, modes, and illumination</t>
+  </si>
+  <si>
+    <t>more stuff on active vs passive, speckle, etc</t>
+  </si>
+  <si>
+    <t>petkie_active_2008</t>
+  </si>
+  <si>
+    <t>http://www.opticsinfobase.org/josaa/abstract.cfm?uri=josaa-29-12-2643</t>
+  </si>
+  <si>
+    <t>http://opticalengineering.spiedigitallibrary.org/article.aspx?articleid=1307605</t>
+  </si>
+  <si>
+    <t>Elimination of speckle and target orientation requirements in millimeter-wave active imaging by modulated multimode mixing illumination</t>
+  </si>
+  <si>
+    <t>more stuff on active, speckle</t>
+  </si>
+  <si>
+    <t>patrick_elimination_2012</t>
+  </si>
+  <si>
+    <t>http://www.opticsinfobase.org/josa/abstract.cfm?uri=josa-66-11-1145</t>
+  </si>
+  <si>
+    <t>Some fundamental properties of speckle</t>
+  </si>
+  <si>
+    <t>good general speckle reference</t>
+  </si>
+  <si>
+    <t>goodman_fundamental_1976</t>
+  </si>
+  <si>
+    <t>http://ieeexplore.ieee.org/xpl/articleDetails.jsp?arnumber=6005340&amp;navigation=1</t>
+  </si>
+  <si>
+    <t>THz Metrology and Instrumentation</t>
+  </si>
+  <si>
+    <t>popovic, grossman</t>
+  </si>
+  <si>
+    <t>popovic_thz_2011</t>
+  </si>
+  <si>
+    <t>technology overview</t>
+  </si>
+  <si>
+    <t>clarke</t>
+  </si>
+  <si>
+    <t>http://scitation.aip.org/content/aip/journal/jap/48/12/10.1063/1.323612</t>
+  </si>
+  <si>
+    <t>Superconductive bolometers for submillimeter wavelengths</t>
+  </si>
+  <si>
+    <t>first Al TES?</t>
+  </si>
+  <si>
+    <t>clarke_superconductive_2008</t>
   </si>
 </sst>
 </file>
@@ -272,11 +648,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -579,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +988,7 @@
     <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +1017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
@@ -638,7 +1032,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -667,7 +1061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -696,7 +1090,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -725,7 +1119,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -754,7 +1148,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -783,7 +1177,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -812,9 +1206,49 @@
         <v>34</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J15" r:id="rId1"/>
+    <hyperlink ref="J12" r:id="rId2"/>
+    <hyperlink ref="J13" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -823,7 +1257,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,12 +1360,533 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="11.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="9" customWidth="1"/>
+    <col min="4" max="5" width="30.7109375" style="6" customWidth="1"/>
+    <col min="6" max="7" width="30.7109375" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2007</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="7">
+        <v>2008</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>2008</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>2011</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>2012</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2013</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2012</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2009</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2013</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1987</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2013</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2013</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2013</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2011</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>1976</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>2007</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>2006</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>2008</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>2009</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>2011</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>1977</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More system comparison details
</commit_message>
<xml_diff>
--- a/support/system-compare.xlsx
+++ b/support/system-compare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="238">
   <si>
     <t>System</t>
   </si>
@@ -114,9 +114,6 @@
     <t>5 m</t>
   </si>
   <si>
-    <t>2.1 cm</t>
-  </si>
-  <si>
     <t>8 FPS</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>0.6 K</t>
   </si>
   <si>
-    <t>8 m</t>
-  </si>
-  <si>
     <t>SPIE Orlando 2010</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
   </si>
   <si>
     <t>0.5 K</t>
-  </si>
-  <si>
-    <t>350 / 20 %</t>
   </si>
   <si>
     <t>7-10 m</t>
@@ -596,13 +587,161 @@
   </si>
   <si>
     <t>clarke_superconductive_2008</t>
+  </si>
+  <si>
+    <t>SPIE Dresden 2013</t>
+  </si>
+  <si>
+    <t>http://spie.org/Documents/ConferencesExhibitions/ERS-ESD13-Final.pdf</t>
+  </si>
+  <si>
+    <t>http://proceedings.spiedigitallibrary.org/volume.aspx?conferenceid=3259&amp;volumeid=16204</t>
+  </si>
+  <si>
+    <t>http://discovery.nationalarchives.gov.uk/SearchUI/Details?uri=C2383503</t>
+  </si>
+  <si>
+    <t>firs passive mmwave imaging system</t>
+  </si>
+  <si>
+    <t>c.r._ditchfield_passive_????</t>
+  </si>
+  <si>
+    <t>Passive detection at Q band</t>
+  </si>
+  <si>
+    <t>Appleby</t>
+  </si>
+  <si>
+    <t>http://rsta.royalsocietypublishing.org/content/362/1815/379.short</t>
+  </si>
+  <si>
+    <t>overview</t>
+  </si>
+  <si>
+    <t>Passive millimetre–wave imaging and how it differs from terahertz imaging</t>
+  </si>
+  <si>
+    <t>appleby_passive_2004</t>
+  </si>
+  <si>
+    <t>http://www.opticsinfobase.org/ol/abstract.cfm?uri=ol-20-16-1716</t>
+  </si>
+  <si>
+    <t>first thz imaging system … time-domain spectroscopy</t>
+  </si>
+  <si>
+    <t>Imaging with terahertz waves</t>
+  </si>
+  <si>
+    <t>hu_imaging_1995</t>
+  </si>
+  <si>
+    <t>http://proceedings.spiedigitallibrary.org/proceeding.aspx?articleid=1270086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Millimetre radar threat level evaluation (MiRTLE) at standoff ranges
+</t>
+  </si>
+  <si>
+    <t>another radar system! But no images yet</t>
+  </si>
+  <si>
+    <t>http://www.mpdigest.com/issue/Articles/2009/aug/mmic/</t>
+  </si>
+  <si>
+    <t>industry article - claims 0.4 K NETD at W band, but no references</t>
+  </si>
+  <si>
+    <t>harmer_millimetre_2011</t>
+  </si>
+  <si>
+    <t>siegel_terahertz_2006, siegel_terahertz_2006</t>
+  </si>
+  <si>
+    <t>siegel - good coherent references</t>
+  </si>
+  <si>
+    <t>http://link.springer.com/article/10.1007/s10762-006-9109-4</t>
+  </si>
+  <si>
+    <t>Progress in focal plane array technologies</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0079672712000183</t>
+  </si>
+  <si>
+    <t>has stuff on mmwave,but no pdf avail</t>
+  </si>
+  <si>
+    <t>rogalski_progress_2012</t>
+  </si>
+  <si>
+    <t>http://link.springer.com/article/10.2478/s11772-013-0110-x</t>
+  </si>
+  <si>
+    <t>Semiconductor detectors and focal plane arrays for far-infrared imaging</t>
+  </si>
+  <si>
+    <t>rogalski_semiconductor_2013</t>
+  </si>
+  <si>
+    <t>http://link.springer.com/article/10.2478%2Fs11772-011-0033-3</t>
+  </si>
+  <si>
+    <t>this is the best of the rogalski articles!</t>
+  </si>
+  <si>
+    <t>rogalski_terahertz_2011</t>
+  </si>
+  <si>
+    <t>Terahertz detectors and focal plane arrays</t>
+  </si>
+  <si>
+    <t>grossman_passive_2010</t>
+  </si>
+  <si>
+    <t>http://www.opticsinfobase.org/ao/abstract.cfm?uri=ao-49-19-E106</t>
+  </si>
+  <si>
+    <t>luukanen_applications_2012</t>
+  </si>
+  <si>
+    <t>http://iopscience.iop.org/1742-6596/400/5/052018/</t>
+  </si>
+  <si>
+    <t>Millilab II</t>
+  </si>
+  <si>
+    <t>4.0 K</t>
+  </si>
+  <si>
+    <t>2.5 cm</t>
+  </si>
+  <si>
+    <t>Millilab readout</t>
+  </si>
+  <si>
+    <t>Low-noise readout of superconducting bolometers based on electrothermal feedback</t>
+  </si>
+  <si>
+    <t>penttila_low-noise_2006</t>
+  </si>
+  <si>
+    <t>http://iopscience.iop.org/0953-2048/19/4/013/</t>
+  </si>
+  <si>
+    <t>idea here is that SQUIDs are finicky and expensive, so develop purely room-temperature approach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +765,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -644,11 +790,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -671,8 +818,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -973,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,9 +1138,10 @@
     <col min="3" max="4" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1017,12 +1170,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1032,7 +1185,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1061,99 +1214,96 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
         <v>58</v>
       </c>
-      <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>48</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
         <v>53</v>
       </c>
-      <c r="I6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>64</v>
@@ -1162,36 +1312,42 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
         <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>226</v>
+      </c>
+      <c r="K7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>231</v>
       </c>
       <c r="F8" t="s">
         <v>31</v>
@@ -1200,45 +1356,70 @@
         <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>232</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>228</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J9" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>68</v>
       </c>
-      <c r="B12" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="J15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>72</v>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" t="s">
+        <v>234</v>
+      </c>
+      <c r="J19" t="s">
+        <v>235</v>
+      </c>
+      <c r="K19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1246,25 +1427,26 @@
     <hyperlink ref="J15" r:id="rId1"/>
     <hyperlink ref="J12" r:id="rId2"/>
     <hyperlink ref="J13" r:id="rId3"/>
+    <hyperlink ref="K8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1279,91 +1461,106 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2">
-        <v>8715</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>44</v>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="3">
+        <v>8900</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>8362</v>
+        <v>8715</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>8022</v>
+        <v>8362</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>8022</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B5">
-        <v>7670</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B6">
+        <v>7670</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
         <v>7309</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>65</v>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D4" r:id="rId5"/>
-    <hyperlink ref="D2" r:id="rId6"/>
-    <hyperlink ref="C6" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D5" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D3" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,51 +1578,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B2" s="7">
         <v>2007</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1433,16 +1630,16 @@
         <v>2008</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1450,10 +1647,10 @@
         <v>2008</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1461,13 +1658,13 @@
         <v>2011</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1475,16 +1672,16 @@
         <v>2012</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1495,85 +1692,85 @@
         <v>2013</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B8" s="7">
         <v>2012</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B9" s="6">
         <v>2009</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B10" s="6">
         <v>2013</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1584,16 +1781,16 @@
         <v>1987</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1604,19 +1801,19 @@
         <v>2013</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>140</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1627,16 +1824,16 @@
         <v>2012</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1647,16 +1844,16 @@
         <v>2013</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1667,13 +1864,13 @@
         <v>2013</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1684,21 +1881,41 @@
         <v>2011</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1706,16 +1923,16 @@
         <v>1976</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1723,16 +1940,16 @@
         <v>2007</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1740,13 +1957,13 @@
         <v>2006</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1754,16 +1971,16 @@
         <v>2008</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1771,16 +1988,16 @@
         <v>2012</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1788,27 +2005,27 @@
         <v>2012</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>128</v>
-      </c>
       <c r="H25" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E26" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1816,16 +2033,16 @@
         <v>2012</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1833,16 +2050,16 @@
         <v>2009</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1850,19 +2067,19 @@
         <v>2011</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>187</v>
-      </c>
       <c r="H29" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1870,23 +2087,150 @@
         <v>1977</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="H30" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>1955</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <v>2004</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>1995</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="F34" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>2007</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>2013</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <v>2011</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H36" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated lit search spreadsheet
</commit_message>
<xml_diff>
--- a/support/system-compare.xlsx
+++ b/support/system-compare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="239">
   <si>
     <t>System</t>
   </si>
@@ -183,16 +183,7 @@
     <t>0.5 K</t>
   </si>
   <si>
-    <t>7-10 m</t>
-  </si>
-  <si>
-    <t>1.05 m diam</t>
-  </si>
-  <si>
     <t>2cm</t>
-  </si>
-  <si>
-    <t>0.1 - 0.4 K</t>
   </si>
   <si>
     <t>10 FPS</t>
@@ -732,6 +723,18 @@
   </si>
   <si>
     <t>idea here is that SQUIDs are finicky and expensive, so develop purely room-temperature approach</t>
+  </si>
+  <si>
+    <t>8.5 m</t>
+  </si>
+  <si>
+    <t>1 m diam</t>
+  </si>
+  <si>
+    <t>Jena II</t>
+  </si>
+  <si>
+    <t>350 GHz / 80 GHz = 23 %</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -1172,10 +1175,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1218,81 +1221,81 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>54</v>
       </c>
       <c r="F4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H4" t="s">
         <v>55</v>
       </c>
-      <c r="G4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
-      </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
+        <v>237</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>235</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>236</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
         <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
         <v>53</v>
@@ -1300,134 +1303,163 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C7">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" t="s">
-        <v>226</v>
-      </c>
-      <c r="K7" t="s">
-        <v>227</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
       <c r="C8">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>231</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
         <v>31</v>
       </c>
       <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>223</v>
+      </c>
+      <c r="K8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>228</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="H8" t="s">
-        <v>232</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="H9" t="s">
+        <v>229</v>
+      </c>
+      <c r="I9" t="s">
         <v>33</v>
       </c>
-      <c r="J8" t="s">
-        <v>228</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J9" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="J9" t="s">
+        <v>225</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>70</v>
+      <c r="A12" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20" t="s">
+        <v>231</v>
+      </c>
+      <c r="J20" t="s">
+        <v>232</v>
+      </c>
+      <c r="K20" t="s">
         <v>233</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>234</v>
-      </c>
-      <c r="J19" t="s">
-        <v>235</v>
-      </c>
-      <c r="K19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J15" r:id="rId1"/>
-    <hyperlink ref="J12" r:id="rId2"/>
-    <hyperlink ref="J13" r:id="rId3"/>
-    <hyperlink ref="K8" r:id="rId4"/>
+    <hyperlink ref="J16" r:id="rId1"/>
+    <hyperlink ref="J13" r:id="rId2"/>
+    <hyperlink ref="J14" r:id="rId3"/>
+    <hyperlink ref="K9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1463,16 +1495,16 @@
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B2" s="3">
         <v>8900</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,16 +1559,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>7309</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1578,51 +1610,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" s="7">
         <v>2007</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1630,16 +1662,16 @@
         <v>2008</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1647,10 +1679,10 @@
         <v>2008</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1658,13 +1690,13 @@
         <v>2011</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1672,16 +1704,16 @@
         <v>2012</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1692,85 +1724,85 @@
         <v>2013</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B8" s="7">
         <v>2012</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" s="6">
         <v>2009</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>103</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B10" s="6">
         <v>2013</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1781,16 +1813,16 @@
         <v>1987</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1801,19 +1833,19 @@
         <v>2013</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1824,16 +1856,16 @@
         <v>2012</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1844,16 +1876,16 @@
         <v>2013</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1864,13 +1896,13 @@
         <v>2013</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1881,16 +1913,16 @@
         <v>2011</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1901,21 +1933,21 @@
         <v>2012</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1923,16 +1955,16 @@
         <v>1976</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1940,16 +1972,16 @@
         <v>2007</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1957,13 +1989,13 @@
         <v>2006</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1971,16 +2003,16 @@
         <v>2008</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1988,16 +2020,16 @@
         <v>2012</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2005,27 +2037,27 @@
         <v>2012</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>125</v>
-      </c>
       <c r="H25" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E26" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2033,16 +2065,16 @@
         <v>2012</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2050,16 +2082,16 @@
         <v>2009</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2067,19 +2099,19 @@
         <v>2011</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>184</v>
-      </c>
       <c r="H29" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2087,19 +2119,19 @@
         <v>1977</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>188</v>
-      </c>
       <c r="H30" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2107,16 +2139,16 @@
         <v>1955</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2124,19 +2156,19 @@
         <v>2004</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2144,24 +2176,24 @@
         <v>1995</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="F34" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2169,13 +2201,13 @@
         <v>2007</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2183,16 +2215,16 @@
         <v>2012</v>
       </c>
       <c r="C36" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>218</v>
-      </c>
       <c r="F36" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2200,13 +2232,13 @@
         <v>2013</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2214,16 +2246,16 @@
         <v>2011</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>